<commit_message>
feat: added eating disorder variables
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/2_0/2_0_yearly_rep.xlsx
+++ b/R/data/dictionaries/core/2_0/2_0_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\LifeCycle\git\analysis_protocols\R\data\dictionaries\core\2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED994D3C-58E8-4B5C-9801-19737719443D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3ACA71-F682-0543-ADE2-4B3E90DC5655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="328">
   <si>
     <t>name</t>
   </si>
@@ -987,6 +987,24 @@
   </si>
   <si>
     <t>Quantity of dogs owned</t>
+  </si>
+  <si>
+    <t>ed_m_</t>
+  </si>
+  <si>
+    <t>an_m_</t>
+  </si>
+  <si>
+    <t>bn_m_</t>
+  </si>
+  <si>
+    <t>Maternal any eating disorder active after the index pregnancy</t>
+  </si>
+  <si>
+    <t>Maternal anorexia nervosa active after the index pregnancy</t>
+  </si>
+  <si>
+    <t>Maternal bulimia nervosa active after the index pregnancy</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1046,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1051,13 +1069,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1077,6 +1106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1540,22 +1573,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG116"/>
+  <dimension ref="A1:BG119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:B72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="169.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="169.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1657,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1639,7 +1672,7 @@
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1652,7 +1685,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1667,7 +1700,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1682,7 +1715,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1697,7 +1730,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1712,7 +1745,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1727,7 +1760,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1742,7 +1775,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1757,7 +1790,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1772,7 +1805,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1787,7 +1820,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1802,7 +1835,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1817,7 +1850,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
@@ -1832,7 +1865,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -1847,7 +1880,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -1862,7 +1895,7 @@
       </c>
       <c r="E17"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
@@ -1877,7 +1910,7 @@
       </c>
       <c r="E18"/>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>27</v>
       </c>
@@ -1892,7 +1925,7 @@
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -1907,7 +1940,7 @@
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1922,7 +1955,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1937,7 +1970,7 @@
       </c>
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1952,7 +1985,7 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1967,7 +2000,7 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -1982,7 +2015,7 @@
       </c>
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
@@ -1997,7 +2030,7 @@
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>312</v>
       </c>
@@ -2012,7 +2045,7 @@
       </c>
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>313</v>
       </c>
@@ -2027,7 +2060,7 @@
       </c>
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>314</v>
       </c>
@@ -2042,7 +2075,7 @@
       </c>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>315</v>
       </c>
@@ -2057,7 +2090,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -2072,7 +2105,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -2087,7 +2120,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -2102,7 +2135,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
@@ -2117,7 +2150,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2165,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>167</v>
       </c>
@@ -2146,7 +2179,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>170</v>
       </c>
@@ -2160,7 +2193,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>172</v>
       </c>
@@ -2174,7 +2207,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>174</v>
       </c>
@@ -2188,7 +2221,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>176</v>
       </c>
@@ -2202,7 +2235,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>178</v>
       </c>
@@ -2216,7 +2249,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>181</v>
       </c>
@@ -2230,7 +2263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>182</v>
       </c>
@@ -2244,7 +2277,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>183</v>
       </c>
@@ -2258,7 +2291,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>184</v>
       </c>
@@ -2272,7 +2305,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>185</v>
       </c>
@@ -2286,7 +2319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>186</v>
       </c>
@@ -2300,7 +2333,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>187</v>
       </c>
@@ -2314,7 +2347,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>188</v>
       </c>
@@ -2328,7 +2361,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>189</v>
       </c>
@@ -2342,7 +2375,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>190</v>
       </c>
@@ -2356,7 +2389,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>191</v>
       </c>
@@ -2370,7 +2403,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>192</v>
       </c>
@@ -2384,7 +2417,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>193</v>
       </c>
@@ -2398,7 +2431,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>194</v>
       </c>
@@ -2412,7 +2445,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>195</v>
       </c>
@@ -2426,7 +2459,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>196</v>
       </c>
@@ -2440,7 +2473,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>197</v>
       </c>
@@ -2454,7 +2487,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>199</v>
       </c>
@@ -2468,7 +2501,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>201</v>
       </c>
@@ -2482,7 +2515,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>202</v>
       </c>
@@ -2496,7 +2529,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>204</v>
       </c>
@@ -2510,7 +2543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>205</v>
       </c>
@@ -2524,7 +2557,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>207</v>
       </c>
@@ -2538,7 +2571,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>208</v>
       </c>
@@ -2552,7 +2585,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>209</v>
       </c>
@@ -2566,7 +2599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>210</v>
       </c>
@@ -2580,7 +2613,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>211</v>
       </c>
@@ -2594,7 +2627,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>212</v>
       </c>
@@ -2608,7 +2641,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>213</v>
       </c>
@@ -2622,7 +2655,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>214</v>
       </c>
@@ -2636,7 +2669,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>215</v>
       </c>
@@ -2650,7 +2683,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>216</v>
       </c>
@@ -2664,7 +2697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>218</v>
       </c>
@@ -2678,7 +2711,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>219</v>
       </c>
@@ -2692,7 +2725,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>220</v>
       </c>
@@ -2706,7 +2739,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>221</v>
       </c>
@@ -2720,7 +2753,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>222</v>
       </c>
@@ -2734,7 +2767,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>223</v>
       </c>
@@ -2748,7 +2781,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>224</v>
       </c>
@@ -2762,7 +2795,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>225</v>
       </c>
@@ -2776,7 +2809,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>226</v>
       </c>
@@ -2790,7 +2823,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>227</v>
       </c>
@@ -2804,7 +2837,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>228</v>
       </c>
@@ -2818,7 +2851,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>229</v>
       </c>
@@ -2832,7 +2865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>231</v>
       </c>
@@ -2846,7 +2879,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>232</v>
       </c>
@@ -2860,7 +2893,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>234</v>
       </c>
@@ -2874,7 +2907,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>161</v>
       </c>
@@ -2888,7 +2921,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>162</v>
       </c>
@@ -2902,7 +2935,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>235</v>
       </c>
@@ -2916,7 +2949,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>237</v>
       </c>
@@ -2930,7 +2963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>238</v>
       </c>
@@ -2944,7 +2977,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>239</v>
       </c>
@@ -2958,7 +2991,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>241</v>
       </c>
@@ -2972,7 +3005,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>164</v>
       </c>
@@ -2986,7 +3019,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>163</v>
       </c>
@@ -3000,7 +3033,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>242</v>
       </c>
@@ -3014,7 +3047,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>165</v>
       </c>
@@ -3028,7 +3061,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>166</v>
       </c>
@@ -3042,7 +3075,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>243</v>
       </c>
@@ -3056,7 +3089,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>245</v>
       </c>
@@ -3070,7 +3103,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>247</v>
       </c>
@@ -3084,7 +3117,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>248</v>
       </c>
@@ -3098,7 +3131,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>250</v>
       </c>
@@ -3112,7 +3145,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>251</v>
       </c>
@@ -3126,7 +3159,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>252</v>
       </c>
@@ -3140,7 +3173,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>255</v>
       </c>
@@ -3154,7 +3187,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>257</v>
       </c>
@@ -3168,7 +3201,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>259</v>
       </c>
@@ -3182,7 +3215,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>261</v>
       </c>
@@ -3196,7 +3229,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>263</v>
       </c>
@@ -3210,7 +3243,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>265</v>
       </c>
@@ -3224,7 +3257,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>268</v>
       </c>
@@ -3238,7 +3271,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>270</v>
       </c>
@@ -3252,7 +3285,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>272</v>
       </c>
@@ -3264,6 +3297,48 @@
       </c>
       <c r="D116" s="5" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D117" s="13" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3277,20 +3352,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A99" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:D137"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="37.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="37.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3304,7 +3381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -3318,7 +3395,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -3332,7 +3409,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -3346,7 +3423,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -3360,7 +3437,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -3374,7 +3451,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3388,7 +3465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -3402,7 +3479,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3416,7 +3493,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3430,7 +3507,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -3444,7 +3521,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -3458,7 +3535,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -3472,7 +3549,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -3486,7 +3563,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -3500,7 +3577,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -3514,7 +3591,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -3528,7 +3605,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -3542,7 +3619,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -3556,7 +3633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -3570,7 +3647,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -3584,7 +3661,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
@@ -3598,7 +3675,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -3612,7 +3689,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3626,7 +3703,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -3640,7 +3717,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -3654,7 +3731,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -3668,7 +3745,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -3682,7 +3759,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
@@ -3696,7 +3773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -3710,7 +3787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>18</v>
       </c>
@@ -3724,7 +3801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
@@ -3738,7 +3815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
@@ -3752,7 +3829,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
@@ -3766,7 +3843,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -3780,7 +3857,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -3794,7 +3871,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
@@ -3808,7 +3885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
@@ -3822,7 +3899,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>20</v>
       </c>
@@ -3836,7 +3913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
@@ -3850,7 +3927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
@@ -3864,7 +3941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>20</v>
       </c>
@@ -3878,7 +3955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
@@ -3892,7 +3969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
@@ -3906,7 +3983,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
@@ -3920,7 +3997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
@@ -3934,7 +4011,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -3948,7 +4025,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
@@ -3962,7 +4039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>21</v>
       </c>
@@ -3976,7 +4053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>21</v>
       </c>
@@ -3990,7 +4067,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>21</v>
       </c>
@@ -4004,7 +4081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>21</v>
       </c>
@@ -4018,7 +4095,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>22</v>
       </c>
@@ -4032,7 +4109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>22</v>
       </c>
@@ -4046,7 +4123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>22</v>
       </c>
@@ -4060,7 +4137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>22</v>
       </c>
@@ -4074,7 +4151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>23</v>
       </c>
@@ -4088,7 +4165,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
@@ -4102,7 +4179,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -4116,7 +4193,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>23</v>
       </c>
@@ -4130,7 +4207,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>23</v>
       </c>
@@ -4144,7 +4221,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>23</v>
       </c>
@@ -4158,7 +4235,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>23</v>
       </c>
@@ -4172,7 +4249,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>23</v>
       </c>
@@ -4186,7 +4263,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
@@ -4200,7 +4277,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>23</v>
       </c>
@@ -4214,7 +4291,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>24</v>
       </c>
@@ -4228,7 +4305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>24</v>
       </c>
@@ -4242,7 +4319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>24</v>
       </c>
@@ -4256,7 +4333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>24</v>
       </c>
@@ -4270,7 +4347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>25</v>
       </c>
@@ -4284,7 +4361,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>25</v>
       </c>
@@ -4298,7 +4375,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>25</v>
       </c>
@@ -4312,7 +4389,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>26</v>
       </c>
@@ -4326,7 +4403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>26</v>
       </c>
@@ -4340,7 +4417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>26</v>
       </c>
@@ -4354,7 +4431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>26</v>
       </c>
@@ -4368,7 +4445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>27</v>
       </c>
@@ -4382,7 +4459,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>27</v>
       </c>
@@ -4396,7 +4473,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>27</v>
       </c>
@@ -4410,7 +4487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>28</v>
       </c>
@@ -4424,7 +4501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>28</v>
       </c>
@@ -4438,7 +4515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>28</v>
       </c>
@@ -4452,7 +4529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>28</v>
       </c>
@@ -4466,7 +4543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>29</v>
       </c>
@@ -4480,7 +4557,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>29</v>
       </c>
@@ -4494,7 +4571,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>30</v>
       </c>
@@ -4508,7 +4585,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
@@ -4522,7 +4599,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>31</v>
       </c>
@@ -4536,7 +4613,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>31</v>
       </c>
@@ -4550,7 +4627,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>32</v>
       </c>
@@ -4564,7 +4641,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>32</v>
       </c>
@@ -4578,7 +4655,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>33</v>
       </c>
@@ -4592,7 +4669,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>33</v>
       </c>
@@ -4606,7 +4683,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>34</v>
       </c>
@@ -4620,7 +4697,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>34</v>
       </c>
@@ -4634,7 +4711,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>312</v>
       </c>
@@ -4648,7 +4725,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>312</v>
       </c>
@@ -4662,7 +4739,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>314</v>
       </c>
@@ -4676,7 +4753,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>314</v>
       </c>
@@ -4690,7 +4767,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>35</v>
       </c>
@@ -4704,7 +4781,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>35</v>
       </c>
@@ -4718,7 +4795,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>36</v>
       </c>
@@ -4732,7 +4809,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>36</v>
       </c>
@@ -4746,7 +4823,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>36</v>
       </c>
@@ -4760,7 +4837,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>36</v>
       </c>
@@ -4774,7 +4851,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>37</v>
       </c>
@@ -4788,7 +4865,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>37</v>
       </c>
@@ -4802,7 +4879,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>161</v>
       </c>
@@ -4816,7 +4893,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>161</v>
       </c>
@@ -4830,7 +4907,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>162</v>
       </c>
@@ -4844,7 +4921,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>162</v>
       </c>
@@ -4858,7 +4935,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>163</v>
       </c>
@@ -4872,7 +4949,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>163</v>
       </c>
@@ -4886,7 +4963,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>163</v>
       </c>
@@ -4900,7 +4977,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>163</v>
       </c>
@@ -4914,7 +4991,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>163</v>
       </c>
@@ -4928,7 +5005,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>164</v>
       </c>
@@ -4942,7 +5019,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>164</v>
       </c>
@@ -4956,7 +5033,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>164</v>
       </c>
@@ -4970,7 +5047,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>164</v>
       </c>
@@ -4984,7 +5061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>164</v>
       </c>
@@ -4998,7 +5075,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>164</v>
       </c>
@@ -5012,7 +5089,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>165</v>
       </c>
@@ -5026,7 +5103,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>165</v>
       </c>
@@ -5040,7 +5117,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>165</v>
       </c>
@@ -5054,7 +5131,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
         <v>166</v>
       </c>
@@ -5068,7 +5145,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
         <v>166</v>
       </c>
@@ -5082,7 +5159,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
         <v>166</v>
       </c>
@@ -5096,7 +5173,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>166</v>
       </c>
@@ -5110,7 +5187,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>166</v>
       </c>
@@ -5122,6 +5199,90 @@
       </c>
       <c r="D131" s="6" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B132" s="11">
+        <v>0</v>
+      </c>
+      <c r="C132" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D132" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B133" s="11">
+        <v>1</v>
+      </c>
+      <c r="C133" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B134" s="11">
+        <v>0</v>
+      </c>
+      <c r="C134" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D134" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B135" s="11">
+        <v>1</v>
+      </c>
+      <c r="C135" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B136" s="11">
+        <v>0</v>
+      </c>
+      <c r="C136" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B137" s="11">
+        <v>1</v>
+      </c>
+      <c r="C137" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>